<commit_message>
Files created during demo
</commit_message>
<xml_diff>
--- a/demo_12_python_file_io/empty_files/empty_worksheet.xlsx
+++ b/demo_12_python_file_io/empty_files/empty_worksheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucf-my.sharepoint.com/personal/le279259_ucf_edu/Documents/Documents/Teaching/QMB6358_Fall_2021/GitRepo/QMB6358F21/demo_13_python_file_io/empty_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucf-my.sharepoint.com/personal/le279259_ucf_edu/Documents/Documents/Teaching/UCF_QMB6358/QMB_6358_Fall_2023/GitHub/QMB6358F23/demo_12_python_file_io/empty_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="11_F25DC773A252ABDACC104846D118639E5ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB3D95D8-0ED1-480F-8CC2-EAD0BC6BFFBB}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="11_F25DC773A252ABDACC104846D118639E5ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E35522A7-25D1-4E54-BC60-DC07D342F458}"/>
   <bookViews>
-    <workbookView xWindow="9768" yWindow="12" windowWidth="13272" windowHeight="12168" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,26 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -360,37 +341,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>